<commit_message>
Se corrigió el problema del descuento de stock en el store y en el update de las ventas
</commit_message>
<xml_diff>
--- a/SCRIPTS/dev/DataEvaluacion.xlsx
+++ b/SCRIPTS/dev/DataEvaluacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\pociones\SCRIPTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\pociones\SCRIPTS\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD79D757-29F5-42E2-81A2-7B711C36CD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F931F709-9D56-48A2-A147-0740742343D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pociones" sheetId="1" r:id="rId1"/>
@@ -1168,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:AMJ58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3955,7 +3955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196549E6-CFB2-4DE5-8478-BD6034641798}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>